<commit_message>
prueba respaldar proyecto 2024
</commit_message>
<xml_diff>
--- a/PortalRh/PortalRh/wwwroot/Templates/PagoTerceros.xlsx
+++ b/PortalRh/PortalRh/wwwroot/Templates/PagoTerceros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integracion\reportes\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPSA\source\repos\Conalep2024\PortalRh\PortalRh\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68074408-7DF2-45CE-9D0F-59060AFEDB78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C4B04C-3B44-408A-9097-5C89973BAA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PagoTerceros" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="SUTCONALEP" sheetId="6" r:id="rId6"/>
     <sheet name="SITACONQROO" sheetId="7" r:id="rId7"/>
     <sheet name="SITEM" sheetId="8" r:id="rId8"/>
+    <sheet name="CREDIFOM" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PagoTerceros!$A$2:$K$3</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="15">
   <si>
     <t>TIPO</t>
   </si>
@@ -82,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">PAGO TERCEROS </t>
+  </si>
+  <si>
+    <t>CREDIFOM</t>
   </si>
 </sst>
 </file>
@@ -91,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -115,6 +119,12 @@
     <font>
       <b/>
       <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -176,28 +186,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -513,45 +533,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="39.5703125" customWidth="1"/>
-    <col min="5" max="11" width="17.85546875" customWidth="1"/>
+    <col min="5" max="11" width="17.85546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -575,22 +597,28 @@
       <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="L2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="17.25">
+      <c r="L5" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:K1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -599,7 +627,113 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24.75" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="19.5" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80915367-B56C-477F-B791-2CA6558050D2}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.25">
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="E3" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE7099B-E8C4-4217-B4E7-89B5C234EEC6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -611,29 +745,29 @@
     <col min="5" max="5" width="17.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.75" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:5" ht="23.25">
+      <c r="A1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -642,16 +776,15 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80915367-B56C-477F-B791-2CA6558050D2}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C7C2E2-F883-41BA-A869-A960538918D1}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -660,17 +793,17 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25">
-      <c r="A1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -685,12 +818,12 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="E3" s="2"/>
+      <c r="E3" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -700,12 +833,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE7099B-E8C4-4217-B4E7-89B5C234EEC6}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFE568A-EE0F-4B8E-8A99-6C3B943FA2E3}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -714,17 +847,17 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25">
-      <c r="A1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -739,12 +872,12 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="E3" s="2"/>
+      <c r="E3" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -754,12 +887,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C7C2E2-F883-41BA-A869-A960538918D1}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F491FC-BA52-4DB2-8F92-EE67B0F880B1}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -768,17 +901,17 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25">
-      <c r="A1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -793,12 +926,12 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="E3" s="2"/>
+      <c r="E3" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -808,12 +941,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFE568A-EE0F-4B8E-8A99-6C3B943FA2E3}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4150A0B6-6939-491C-81A8-F0C702E63DBC}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -822,17 +955,17 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -847,12 +980,12 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="E3" s="2"/>
+      <c r="E3" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -862,12 +995,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F491FC-BA52-4DB2-8F92-EE67B0F880B1}">
-  <dimension ref="A1:E3"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510E9E0D-78D3-4494-813D-75E7566ECAE1}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -876,17 +1009,17 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25">
-      <c r="A1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -901,71 +1034,15 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4150A0B6-6939-491C-81A8-F0C702E63DBC}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="23.25">
-      <c r="A1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="E3" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>